<commit_message>
Updates Made in this commit: .) Refactoring new keys map
Trying to do in this update:
.) Fix updating Mysql database with foodInfo search results.

Errors:
.)

Next To Do:
.) scrollBar_Down to bottom doesn't scroll all the way to the bottom when adding a meal.

Need to update:
.) ScrollBar_Down BTN incorporated & into add new meal functionality.

.) Delete folder in path: "src/Resources/Database Docs/New Setup3" if not needed.

.) Edit_Ingredients_Types_Screen() - doesnt remove space in ingredientType name provided when adding it to the db - check Edit_Ingredient_Stores_Screen() too.

.) Cant Update ingredient price if its in a meal.

.) Any edits to ingredients needs to update meals
</commit_message>
<xml_diff>
--- a/src/App_Code/Objects/API/Nutritionix/Resources/Nutritionix API v2 - Full Nutrient USDA Field Mapping [PUBLIC].xlsx
+++ b/src/App_Code/Objects/API/Nutritionix/Resources/Nutritionix API v2 - Full Nutrient USDA Field Mapping [PUBLIC].xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DonTy\Dropbox\0.) Coding\Gym_App\src\Tests\HTTP\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DonTy\Dropbox\0.) Coding\Gym_App\src\App_Code\Objects\API\Nutritionix\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCE282F-5173-4B0A-B635-D3B792821C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08474534-8AAF-4926-8128-961704828C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68010" yWindow="8040" windowWidth="12585" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="66045" yWindow="0" windowWidth="14370" windowHeight="20955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes for natural endpoint" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="283">
   <si>
     <t>attr_id</t>
   </si>
@@ -76,9 +76,6 @@
     <t>CA</t>
   </si>
   <si>
-    <t>Calcium, Ca</t>
-  </si>
-  <si>
     <t>mg</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>FE</t>
   </si>
   <si>
-    <t>Iron, Fe</t>
-  </si>
-  <si>
     <t>FIBTG</t>
   </si>
   <si>
@@ -241,9 +235,6 @@
     <t>CHOCAL</t>
   </si>
   <si>
-    <t>Vitamin D3 (cholecalciferol)</t>
-  </si>
-  <si>
     <t>CHOLN</t>
   </si>
   <si>
@@ -259,9 +250,6 @@
     <t>CU</t>
   </si>
   <si>
-    <t>Copper, Cu</t>
-  </si>
-  <si>
     <t>CYS_G</t>
   </si>
   <si>
@@ -277,9 +265,6 @@
     <t>ERGCAL</t>
   </si>
   <si>
-    <t>Vitamin D2 (ergocalciferol)</t>
-  </si>
-  <si>
     <t>F10D0</t>
   </si>
   <si>
@@ -640,9 +625,6 @@
     <t>MG</t>
   </si>
   <si>
-    <t>Magnesium, Mg</t>
-  </si>
-  <si>
     <t>MK4</t>
   </si>
   <si>
@@ -664,12 +646,6 @@
     <t>NULL</t>
   </si>
   <si>
-    <t>Vitamin E, added</t>
-  </si>
-  <si>
-    <t>Vitamin B-12, added</t>
-  </si>
-  <si>
     <t>Adjusted Protein</t>
   </si>
   <si>
@@ -691,9 +667,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>Phosphorus, P</t>
-  </si>
-  <si>
     <t>PANTAC</t>
   </si>
   <si>
@@ -733,9 +706,6 @@
     <t>SE</t>
   </si>
   <si>
-    <t>Selenium, Se</t>
-  </si>
-  <si>
     <t>SER_G</t>
   </si>
   <si>
@@ -787,9 +757,6 @@
     <t>TOCPHA</t>
   </si>
   <si>
-    <t>Vitamin E (alpha-tocopherol)</t>
-  </si>
-  <si>
     <t>TOCPHB</t>
   </si>
   <si>
@@ -853,18 +820,12 @@
     <t>VITC</t>
   </si>
   <si>
-    <t>Vitamin C, total ascorbic acid</t>
-  </si>
-  <si>
     <t>Vitamin D (D2 + D3)</t>
   </si>
   <si>
     <t>VITK1</t>
   </si>
   <si>
-    <t>Vitamin K (phylloquinone)</t>
-  </si>
-  <si>
     <t>VITK1D</t>
   </si>
   <si>
@@ -880,9 +841,6 @@
     <t>ZN</t>
   </si>
   <si>
-    <t>Zinc, Zn</t>
-  </si>
-  <si>
     <t>TOCTRA</t>
   </si>
   <si>
@@ -911,6 +869,42 @@
   </si>
   <si>
     <t>https://www.fda.gov/downloads/Food/GuidanceRegulation/GuidanceDocumentsRegulatoryInformation/LabelingNutrition/UCM513817.pdf</t>
+  </si>
+  <si>
+    <t>Calcium</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitamin D3 </t>
+  </si>
+  <si>
+    <t>Copper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitamin D2 </t>
+  </si>
+  <si>
+    <t>Magnesium</t>
+  </si>
+  <si>
+    <t>Vitamin E</t>
+  </si>
+  <si>
+    <t>Phosphorus</t>
+  </si>
+  <si>
+    <t>Zinc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitamin K </t>
+  </si>
+  <si>
+    <t>Vitamin C</t>
+  </si>
+  <si>
+    <t>Selenium</t>
   </si>
 </sst>
 </file>
@@ -1299,15 +1293,15 @@
   <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D206" sqref="D206"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="7.5703125" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1339,10 +1333,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1353,13 +1347,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1370,13 +1364,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1387,13 +1381,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1404,13 +1398,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1421,13 +1415,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1438,13 +1432,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1455,13 +1449,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>272</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1472,13 +1466,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1489,13 +1483,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1506,13 +1500,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1523,13 +1517,13 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1540,13 +1534,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1557,13 +1551,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1574,13 +1568,13 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1591,13 +1585,13 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1608,13 +1602,13 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1625,13 +1619,13 @@
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1642,13 +1636,13 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1659,13 +1653,13 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1676,13 +1670,13 @@
         <v>0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1693,13 +1687,13 @@
         <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1710,13 +1704,13 @@
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1727,13 +1721,13 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1744,13 +1738,13 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1761,13 +1755,13 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>61</v>
+        <v>273</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1778,13 +1772,13 @@
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1795,13 +1789,13 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1812,13 +1806,13 @@
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>67</v>
+        <v>274</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1829,13 +1823,13 @@
         <v>0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1846,13 +1840,13 @@
         <v>0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1863,13 +1857,13 @@
         <v>0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>73</v>
+        <v>275</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1880,13 +1874,13 @@
         <v>0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D34" s="4">
         <v>0.41666666666666669</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1897,13 +1891,13 @@
         <v>0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D35" s="4">
         <v>0.5</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1914,13 +1908,13 @@
         <v>0</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D36" s="4">
         <v>0.54166666666666663</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1931,13 +1925,13 @@
         <v>0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D37" s="4">
         <v>0.58333333333333337</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1948,13 +1942,13 @@
         <v>0</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D38" s="4">
         <v>0.58402777777777781</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1965,13 +1959,13 @@
         <v>0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D39" s="4">
         <v>0.625</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1982,13 +1976,13 @@
         <v>0</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D40" s="4">
         <v>0.62569444444444444</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1999,13 +1993,13 @@
         <v>0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D41" s="4">
         <v>0.66666666666666663</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2016,13 +2010,13 @@
         <v>0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2033,13 +2027,13 @@
         <v>0</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2050,13 +2044,13 @@
         <v>0</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2067,13 +2061,13 @@
         <v>0</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D45" s="4">
         <v>0.70833333333333337</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2084,13 +2078,13 @@
         <v>0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D46" s="4">
         <v>0.70902777777777781</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2101,13 +2095,13 @@
         <v>0</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D47" s="4">
         <v>0.75</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2118,13 +2112,13 @@
         <v>0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2135,13 +2129,13 @@
         <v>0</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -2152,13 +2146,13 @@
         <v>0</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2169,13 +2163,13 @@
         <v>0</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2186,13 +2180,13 @@
         <v>0</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2203,13 +2197,13 @@
         <v>0</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2220,13 +2214,13 @@
         <v>0</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2237,13 +2231,13 @@
         <v>0</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2254,13 +2248,13 @@
         <v>0</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2271,13 +2265,13 @@
         <v>0</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2288,13 +2282,13 @@
         <v>0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2305,13 +2299,13 @@
         <v>0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D59" s="4">
         <v>0.75277777777777777</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2322,13 +2316,13 @@
         <v>0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D60" s="4">
         <v>0.83333333333333337</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2339,13 +2333,13 @@
         <v>0</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D61" s="4">
         <v>0.83402777777777781</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -2356,13 +2350,13 @@
         <v>0</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2373,13 +2367,13 @@
         <v>0</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -2390,13 +2384,13 @@
         <v>0</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2407,13 +2401,13 @@
         <v>0</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2424,13 +2418,13 @@
         <v>0</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2441,13 +2435,13 @@
         <v>0</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2458,13 +2452,13 @@
         <v>0</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2475,13 +2469,13 @@
         <v>0</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D69" s="4">
         <v>0.87847222222222221</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2492,13 +2486,13 @@
         <v>0</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D70" s="4">
         <v>0.91666666666666663</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2509,13 +2503,13 @@
         <v>0</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2526,13 +2520,13 @@
         <v>0</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D72" s="4">
         <v>0.9194444444444444</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2543,13 +2537,13 @@
         <v>0</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2560,13 +2554,13 @@
         <v>0</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2577,13 +2571,13 @@
         <v>0</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D75" s="5">
         <v>1</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2594,13 +2588,13 @@
         <v>0</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2611,13 +2605,13 @@
         <v>0</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D77" s="4">
         <v>0.16666666666666666</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2628,13 +2622,13 @@
         <v>0</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D78" s="4">
         <v>0.25</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2645,13 +2639,13 @@
         <v>0</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D79" s="4">
         <v>0.33333333333333331</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2662,13 +2656,13 @@
         <v>0</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2679,13 +2673,13 @@
         <v>0</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -2696,13 +2690,13 @@
         <v>0</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2713,13 +2707,13 @@
         <v>0</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -2730,13 +2724,13 @@
         <v>0</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2747,13 +2741,13 @@
         <v>0</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -2764,13 +2758,13 @@
         <v>0</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2781,13 +2775,13 @@
         <v>0</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2798,13 +2792,13 @@
         <v>0</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2815,13 +2809,13 @@
         <v>0</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2832,13 +2826,13 @@
         <v>0</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -2849,13 +2843,13 @@
         <v>0</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -2866,13 +2860,13 @@
         <v>0</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2883,13 +2877,13 @@
         <v>0</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -2900,13 +2894,13 @@
         <v>0</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2917,13 +2911,13 @@
         <v>0</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2934,13 +2928,13 @@
         <v>0</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2951,13 +2945,13 @@
         <v>0</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2968,13 +2962,13 @@
         <v>0</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2985,13 +2979,13 @@
         <v>0</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -3002,13 +2996,13 @@
         <v>0</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -3019,13 +3013,13 @@
         <v>0</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -3036,13 +3030,13 @@
         <v>0</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -3053,13 +3047,13 @@
         <v>0</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -3070,13 +3064,13 @@
         <v>0</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>194</v>
+        <v>276</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -3087,13 +3081,13 @@
         <v>0</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -3104,13 +3098,13 @@
         <v>0</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -3121,13 +3115,13 @@
         <v>0</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -3138,13 +3132,13 @@
         <v>0</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>202</v>
+        <v>277</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -3155,13 +3149,13 @@
         <v>0</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>203</v>
+        <v>250</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -3172,13 +3166,13 @@
         <v>0</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -3189,13 +3183,13 @@
         <v>0</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -3206,13 +3200,13 @@
         <v>0</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -3223,13 +3217,13 @@
         <v>0</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -3240,13 +3234,13 @@
         <v>0</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -3257,13 +3251,13 @@
         <v>0</v>
       </c>
       <c r="C115" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D115" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="E115" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -3274,13 +3268,13 @@
         <v>0</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>211</v>
+        <v>278</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -3291,13 +3285,13 @@
         <v>0</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -3308,13 +3302,13 @@
         <v>0</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -3325,13 +3319,13 @@
         <v>0</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -3342,13 +3336,13 @@
         <v>0</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -3359,13 +3353,13 @@
         <v>0</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -3376,13 +3370,13 @@
         <v>0</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -3393,13 +3387,13 @@
         <v>0</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>225</v>
+        <v>282</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -3410,13 +3404,13 @@
         <v>0</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -3427,13 +3421,13 @@
         <v>0</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -3444,13 +3438,13 @@
         <v>0</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -3461,13 +3455,13 @@
         <v>0</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -3478,13 +3472,13 @@
         <v>0</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -3495,13 +3489,13 @@
         <v>0</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -3512,13 +3506,13 @@
         <v>0</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -3529,13 +3523,13 @@
         <v>0</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -3546,13 +3540,13 @@
         <v>0</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>243</v>
+        <v>277</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -3563,13 +3557,13 @@
         <v>0</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -3580,13 +3574,13 @@
         <v>0</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -3597,13 +3591,13 @@
         <v>0</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -3614,13 +3608,13 @@
         <v>0</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -3631,13 +3625,13 @@
         <v>0</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -3648,13 +3642,13 @@
         <v>0</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -3665,13 +3659,13 @@
         <v>0</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -3682,13 +3676,13 @@
         <v>0</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -3699,13 +3693,13 @@
         <v>0</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -3716,13 +3710,13 @@
         <v>0</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -3733,13 +3727,13 @@
         <v>0</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>265</v>
+        <v>281</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -3750,13 +3744,13 @@
         <v>0</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -3767,13 +3761,13 @@
         <v>0</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -3784,13 +3778,13 @@
         <v>0</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -3801,13 +3795,13 @@
         <v>0</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -3818,13 +3812,13 @@
         <v>0</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="15.75" customHeight="1">
@@ -3833,13 +3827,13 @@
       </c>
       <c r="B149" s="7"/>
       <c r="C149" s="6" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="E149" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="15.75" customHeight="1">
@@ -3848,13 +3842,13 @@
       </c>
       <c r="B150" s="7"/>
       <c r="C150" s="6" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="E150" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="15.75" customHeight="1">
@@ -3863,13 +3857,13 @@
       </c>
       <c r="B151" s="7"/>
       <c r="C151" s="6" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="E151" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="15.75" customHeight="1">
@@ -3878,18 +3872,19 @@
       </c>
       <c r="B152" s="7"/>
       <c r="C152" s="6" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="E152" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3910,10 +3905,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>